<commit_message>
MAJOR CHANGES MMsoil reformulated to be compliant with paper equations Inf from surface to first soil layer computed and exported Exf from soil exported and plotted in TS Clear distinction from infiltration (surface to soil) and percolation (from bottom of soil layer to percolation zone)
</commit_message>
<xml_diff>
--- a/trunk/MARMITESutilities/MM_XLSstuff/POND_EvaporationCorrection.xlsx
+++ b/trunk/MARMITESutilities/MM_XLSstuff/POND_EvaporationCorrection.xlsx
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,8 +1206,8 @@
         <v>22.536955674275141</v>
       </c>
       <c r="H8" s="2">
-        <f>C8*D8*B8*$K$3*B8^2/100^2/10</f>
-        <v>22.536955674275141</v>
+        <f>C8*D8*$K$3*B8^3/100^2/10</f>
+        <v>22.536955674275138</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>2.2536955674275137E-2</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9:H10" si="3">C9*D9*B9*$K$3*B9^2/100^2/10</f>
+        <f t="shared" ref="H9:H10" si="3">C9*D9*$K$3*B9^3/100^2/10</f>
         <v>2.2536955674275137E-2</v>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="3"/>
-        <v>2.8171194592843927</v>
+        <v>2.8171194592843922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>